<commit_message>
Refinamento dos dados e criação da Baseline
</commit_message>
<xml_diff>
--- a/AnaliseRepositorios.xlsx
+++ b/AnaliseRepositorios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab_6_EX2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4843D0-AC60-41BE-A070-72DCE0AD667A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A3CE7F-F6C0-433E-9B38-4DAF4BB08FA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Analise dos Dados" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Analise dos Dados'!$A$1:$H$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Analise dos Dados'!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="191">
   <si>
     <t>Nome/Dono</t>
   </si>
@@ -577,64 +577,25 @@
     <t xml:space="preserve">	112501</t>
   </si>
   <si>
-    <t xml:space="preserve">	2865</t>
-  </si>
-  <si>
     <t xml:space="preserve">	669</t>
   </si>
   <si>
-    <t xml:space="preserve">	29880</t>
-  </si>
-  <si>
     <t xml:space="preserve">	659354</t>
   </si>
   <si>
-    <t xml:space="preserve">	3972</t>
-  </si>
-  <si>
     <t xml:space="preserve">	4068</t>
   </si>
   <si>
-    <t xml:space="preserve">	3933</t>
-  </si>
-  <si>
     <t xml:space="preserve">	1648</t>
   </si>
   <si>
-    <t xml:space="preserve">	51569</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	1645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	740970</t>
-  </si>
-  <si>
     <t xml:space="preserve">	11608</t>
   </si>
   <si>
-    <t xml:space="preserve">	94773</t>
-  </si>
-  <si>
     <t xml:space="preserve">	390</t>
   </si>
   <si>
-    <t xml:space="preserve">	291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	755749</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	1893</t>
-  </si>
-  <si>
     <t xml:space="preserve">	355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	29451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	4561</t>
   </si>
   <si>
     <t xml:space="preserve">	16377</t>
@@ -1204,19 +1165,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2630,14 +2591,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6F2C9A-A1CA-4FB1-A1B4-E026446CB290}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16:U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
@@ -2651,7 +2613,7 @@
     <col min="21" max="21" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A1)</f>
         <v>Nome/Dono</v>
@@ -2691,10 +2653,10 @@
         <v>179</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A5)</f>
         <v>bbcmicrobit/micropython</v>
@@ -2728,7 +2690,7 @@
         <v>42223</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A10)</f>
         <v>python/typed_ast</v>
@@ -2762,7 +2724,7 @@
         <v>42416</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A12)</f>
         <v>gvanrossum/path-pep</v>
@@ -2796,7 +2758,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CLEAN(RepositoriosPython!A29)</f>
         <v>gvanrossum/mirror-cwi-stdwin</v>
@@ -2830,7 +2792,7 @@
         <v>43372</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A31)</f>
         <v>gvanrossum/memcached</v>
@@ -2864,7 +2826,7 @@
         <v>43457</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A37)</f>
         <v>gvanrossum/PackCC</v>
@@ -2898,7 +2860,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A38)</f>
         <v>gvanrossum/ctok</v>
@@ -2932,7 +2894,7 @@
         <v>43638</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A13)</f>
         <v>gvanrossum/Pyjion</v>
@@ -2966,7 +2928,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CLEAN(RepositoriosPython!A11)</f>
         <v>JukkaL/mypy-website</v>
@@ -3000,7 +2962,7 @@
         <v>42440</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CLEAN(RepositoriosPython!A18)</f>
         <v>gvanrossum/gvanrossum.github.io</v>
@@ -3034,7 +2996,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CLEAN(RepositoriosPython!A23)</f>
         <v>gvanrossum/pythonlabs</v>
@@ -3068,7 +3030,7 @@
         <v>42890</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CLEAN(RepositoriosPython!A16)</f>
         <v>python/overload-sig</v>
@@ -3102,7 +3064,7 @@
         <v>42599</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A39)</f>
         <v>willingc/test-581</v>
@@ -3136,7 +3098,7 @@
         <v>43644</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A2)</f>
         <v>python/mypy</v>
@@ -3170,7 +3132,7 @@
         <v>41250</v>
       </c>
       <c r="I15" s="2">
-        <f>VALUE(CLEAN(M15))</f>
+        <f t="shared" ref="I15:I25" si="0">VALUE(CLEAN(M15))</f>
         <v>112501</v>
       </c>
       <c r="K15" s="9">
@@ -3185,518 +3147,518 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A3)</f>
-        <v>gvanrossum/500lines</v>
+        <f>CLEAN(RepositoriosPython!A4)</f>
+        <v>gvanrossum/ballot-box</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B3)</f>
-        <v>https://github.com/gvanrossum/500lines</v>
+        <f>CLEAN(RepositoriosPython!B4)</f>
+        <v>https://github.com/gvanrossum/ballot-box</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C3)</f>
+        <f>CLEAN(RepositoriosPython!C4)</f>
         <v>Python</v>
       </c>
       <c r="D16" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D3))</f>
-        <v>208</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D4))</f>
+        <v>8</v>
       </c>
       <c r="E16" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E3))</f>
-        <v>13</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E4))</f>
+        <v>2</v>
       </c>
       <c r="F16" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F3))</f>
-        <v>35</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F4))</f>
+        <v>4</v>
       </c>
       <c r="G16" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G3))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G4))</f>
         <v>0</v>
       </c>
       <c r="H16" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H3,1,11)))</f>
-        <v>41695</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H4,1,11)))</f>
+        <v>42076</v>
       </c>
       <c r="I16" s="2">
-        <f>VALUE(CLEAN(M16))</f>
-        <v>2865</v>
+        <f t="shared" si="0"/>
+        <v>669</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" ref="K16:K39" si="0">_xlfn.DAYS("14/03/2020",H16)</f>
-        <v>2209</v>
+        <f t="shared" ref="K16:K25" si="1">_xlfn.DAYS("14/03/2020",H16)</f>
+        <v>1828</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" ref="L16:L39" si="1">G16/K16</f>
+        <f t="shared" ref="L16:L25" si="2">G16/K16</f>
         <v>0</v>
       </c>
       <c r="M16" t="s">
         <v>181</v>
       </c>
+      <c r="O16" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A4)</f>
-        <v>gvanrossum/ballot-box</v>
+        <f>CLEAN(RepositoriosPython!A7)</f>
+        <v>fake-python/cpython</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B4)</f>
-        <v>https://github.com/gvanrossum/ballot-box</v>
+        <f>CLEAN(RepositoriosPython!B7)</f>
+        <v>https://github.com/fake-python/cpython</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C4)</f>
+        <f>CLEAN(RepositoriosPython!C7)</f>
         <v>Python</v>
       </c>
       <c r="D17" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D4))</f>
-        <v>8</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D7))</f>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E4))</f>
-        <v>2</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E7))</f>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F4))</f>
-        <v>4</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F7))</f>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G4))</f>
-        <v>0</v>
+        <f>VALUE(CLEAN(RepositoriosPython!G7))</f>
+        <v>6</v>
       </c>
       <c r="H17" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H4,1,11)))</f>
-        <v>42076</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H7,1,11)))</f>
+        <v>42313</v>
       </c>
       <c r="I17" s="2">
-        <f>VALUE(CLEAN(M17))</f>
-        <v>669</v>
+        <f t="shared" si="0"/>
+        <v>659354</v>
       </c>
       <c r="K17" s="9">
-        <f t="shared" si="0"/>
-        <v>1828</v>
+        <f t="shared" si="1"/>
+        <v>1591</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3.771213073538655E-3</v>
       </c>
       <c r="M17" t="s">
         <v>182</v>
       </c>
+      <c r="O17" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="S17" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="T17" s="14"/>
+      <c r="U17" s="7" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A6)</f>
-        <v>gvanrossum/asyncio</v>
+        <f>CLEAN(RepositoriosPython!A9)</f>
+        <v>edreamleo/make-stub-files</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B6)</f>
-        <v>https://github.com/gvanrossum/asyncio</v>
+        <f>CLEAN(RepositoriosPython!B9)</f>
+        <v>https://github.com/edreamleo/make-stub-files</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C6)</f>
+        <f>CLEAN(RepositoriosPython!C9)</f>
         <v>Python</v>
       </c>
       <c r="D18" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D6))</f>
-        <v>9</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D9))</f>
+        <v>20</v>
       </c>
       <c r="E18" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E6))</f>
-        <v>1</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E9))</f>
+        <v>3</v>
       </c>
       <c r="F18" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F6))</f>
-        <v>2</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F9))</f>
+        <v>3</v>
       </c>
       <c r="G18" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G6))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G9))</f>
         <v>0</v>
       </c>
       <c r="H18" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H6,1,11)))</f>
-        <v>42272</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H9,1,11)))</f>
+        <v>42395</v>
       </c>
       <c r="I18" s="2">
-        <f>VALUE(CLEAN(M18))</f>
-        <v>29880</v>
+        <f t="shared" si="0"/>
+        <v>4068</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" si="0"/>
-        <v>1632</v>
+        <f t="shared" si="1"/>
+        <v>1509</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M18" t="s">
         <v>183</v>
       </c>
+      <c r="O18" s="7" t="str">
+        <f>D1</f>
+        <v>Nº de Estrelas</v>
+      </c>
+      <c r="P18" s="7" t="str">
+        <f>E1</f>
+        <v>Nº de Watchers</v>
+      </c>
+      <c r="Q18" s="7" t="str">
+        <f>F1</f>
+        <v>Nº de Forks</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="S18" s="7" t="str">
+        <f>G1</f>
+        <v>Nº de Releases</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A7)</f>
-        <v>fake-python/cpython</v>
+        <f>CLEAN(RepositoriosPython!A17)</f>
+        <v>ilevkivskyi/com2ann</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B7)</f>
-        <v>https://github.com/fake-python/cpython</v>
+        <f>CLEAN(RepositoriosPython!B17)</f>
+        <v>https://github.com/ilevkivskyi/com2ann</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C7)</f>
+        <f>CLEAN(RepositoriosPython!C17)</f>
         <v>Python</v>
       </c>
       <c r="D19" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D7))</f>
-        <v>3</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D17))</f>
+        <v>50</v>
       </c>
       <c r="E19" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E7))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!E17))</f>
+        <v>6</v>
+      </c>
+      <c r="F19" s="2">
+        <f>VALUE(CLEAN(RepositoriosPython!F17))</f>
         <v>1</v>
       </c>
-      <c r="F19" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F7))</f>
-        <v>0</v>
-      </c>
       <c r="G19" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G7))</f>
-        <v>6</v>
+        <f>VALUE(CLEAN(RepositoriosPython!G17))</f>
+        <v>0</v>
       </c>
       <c r="H19" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H7,1,11)))</f>
-        <v>42313</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H17,1,11)))</f>
+        <v>42622</v>
       </c>
       <c r="I19" s="2">
-        <f>VALUE(CLEAN(M19))</f>
-        <v>659354</v>
+        <f t="shared" si="0"/>
+        <v>1648</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" si="0"/>
-        <v>1591</v>
+        <f t="shared" si="1"/>
+        <v>1282</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="1"/>
-        <v>3.771213073538655E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M19" t="s">
         <v>184</v>
       </c>
+      <c r="O19" s="8">
+        <f>D28</f>
+        <v>49</v>
+      </c>
+      <c r="P19" s="8">
+        <f>E28</f>
+        <v>6</v>
+      </c>
+      <c r="Q19" s="8">
+        <f>F28</f>
+        <v>3</v>
+      </c>
+      <c r="R19" s="8">
+        <f>I28</f>
+        <v>1648</v>
+      </c>
+      <c r="S19" s="8">
+        <f>G28</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="8">
+        <f>L28</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="8">
+        <f>H28</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A8)</f>
-        <v>gvanrossum/pyxl3</v>
+        <f>CLEAN(RepositoriosPython!A22)</f>
+        <v>neogeny/TatSu</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B8)</f>
-        <v>https://github.com/gvanrossum/pyxl3</v>
+        <f>CLEAN(RepositoriosPython!B22)</f>
+        <v>https://github.com/neogeny/TatSu</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C8)</f>
+        <f>CLEAN(RepositoriosPython!C22)</f>
         <v>Python</v>
       </c>
       <c r="D20" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D8))</f>
-        <v>107</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D22))</f>
+        <v>146</v>
       </c>
       <c r="E20" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E8))</f>
-        <v>12</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E22))</f>
+        <v>13</v>
       </c>
       <c r="F20" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F8))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!F22))</f>
+        <v>34</v>
+      </c>
+      <c r="G20" s="2">
+        <f>VALUE(CLEAN(RepositoriosPython!G22))</f>
         <v>13</v>
       </c>
-      <c r="G20" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G8))</f>
-        <v>0</v>
-      </c>
       <c r="H20" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H8,1,11)))</f>
-        <v>42384</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H22,1,11)))</f>
+        <v>42857</v>
       </c>
       <c r="I20" s="2">
-        <f>VALUE(CLEAN(M20))</f>
-        <v>3972</v>
+        <f t="shared" si="0"/>
+        <v>11608</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" si="0"/>
-        <v>1520</v>
+        <f t="shared" si="1"/>
+        <v>1047</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.2416427889207259E-2</v>
       </c>
       <c r="M20" t="s">
         <v>185</v>
       </c>
-      <c r="O20" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A9)</f>
-        <v>edreamleo/make-stub-files</v>
+        <f>CLEAN(RepositoriosPython!A25)</f>
+        <v>gvanrossum/mypy-dummy</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B9)</f>
-        <v>https://github.com/edreamleo/make-stub-files</v>
+        <f>CLEAN(RepositoriosPython!B25)</f>
+        <v>https://github.com/gvanrossum/mypy-dummy</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C9)</f>
+        <f>CLEAN(RepositoriosPython!C25)</f>
         <v>Python</v>
       </c>
       <c r="D21" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D9))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!D25))</f>
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <f>VALUE(CLEAN(RepositoriosPython!E25))</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
+        <f>VALUE(CLEAN(RepositoriosPython!F25))</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <f>VALUE(CLEAN(RepositoriosPython!G25))</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H25,1,11)))</f>
+        <v>42978</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K21" s="9">
+        <f t="shared" si="1"/>
+        <v>926</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
         <v>20</v>
-      </c>
-      <c r="E21" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E9))</f>
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F9))</f>
-        <v>3</v>
-      </c>
-      <c r="G21" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G9))</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H9,1,11)))</f>
-        <v>42395</v>
-      </c>
-      <c r="I21" s="2">
-        <f>VALUE(CLEAN(M21))</f>
-        <v>4068</v>
-      </c>
-      <c r="K21" s="9">
-        <f t="shared" si="0"/>
-        <v>1509</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M21" t="s">
-        <v>186</v>
-      </c>
-      <c r="O21" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="S21" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="T21" s="13"/>
-      <c r="U21" s="7" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A14)</f>
-        <v>ilevkivskyi/peps</v>
+        <f>CLEAN(RepositoriosPython!A26)</f>
+        <v>gvanrossum/pep550</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B14)</f>
-        <v>https://github.com/ilevkivskyi/peps</v>
+        <f>CLEAN(RepositoriosPython!B26)</f>
+        <v>https://github.com/gvanrossum/pep550</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C14)</f>
+        <f>CLEAN(RepositoriosPython!C26)</f>
         <v>Python</v>
       </c>
       <c r="D22" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D14))</f>
-        <v>0</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D26))</f>
+        <v>7</v>
       </c>
       <c r="E22" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E14))</f>
-        <v>5</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E26))</f>
+        <v>3</v>
       </c>
       <c r="F22" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F14))</f>
-        <v>0</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F26))</f>
+        <v>1</v>
       </c>
       <c r="G22" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G14))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G26))</f>
         <v>0</v>
       </c>
       <c r="H22" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H14,1,11)))</f>
-        <v>42565</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H26,1,11)))</f>
+        <v>42983</v>
       </c>
       <c r="I22" s="2">
-        <f>VALUE(CLEAN(M22))</f>
-        <v>3933</v>
+        <f t="shared" si="0"/>
+        <v>390</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="0"/>
-        <v>1339</v>
+        <f t="shared" si="1"/>
+        <v>921</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>187</v>
-      </c>
-      <c r="O22" s="7" t="str">
-        <f>D1</f>
-        <v>Nº de Estrelas</v>
-      </c>
-      <c r="P22" s="7" t="str">
-        <f>E1</f>
-        <v>Nº de Watchers</v>
-      </c>
-      <c r="Q22" s="7" t="str">
-        <f>F1</f>
-        <v>Nº de Forks</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="S22" s="7" t="str">
-        <f>G1</f>
-        <v>Nº de Releases</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A15)</f>
-        <v>phouse512/peps</v>
+        <f>CLEAN(RepositoriosPython!A33)</f>
+        <v>python/mypy_extensions</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B15)</f>
-        <v>https://github.com/phouse512/peps</v>
+        <f>CLEAN(RepositoriosPython!B33)</f>
+        <v>https://github.com/python/mypy_extensions</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C15)</f>
+        <f>CLEAN(RepositoriosPython!C33)</f>
         <v>Python</v>
       </c>
       <c r="D23" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D15))</f>
-        <v>5</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D33))</f>
+        <v>68</v>
       </c>
       <c r="E23" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E15))</f>
-        <v>2</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E33))</f>
+        <v>13</v>
       </c>
       <c r="F23" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F15))</f>
-        <v>4</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F33))</f>
+        <v>12</v>
       </c>
       <c r="G23" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G15))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G33))</f>
         <v>0</v>
       </c>
       <c r="H23" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H15,1,11)))</f>
-        <v>42591</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H33,1,11)))</f>
+        <v>43479</v>
       </c>
       <c r="I23" s="2">
-        <f>VALUE(CLEAN(M23))</f>
-        <v>3933</v>
+        <f t="shared" si="0"/>
+        <v>355</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="0"/>
-        <v>1313</v>
+        <f t="shared" si="1"/>
+        <v>425</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23" t="s">
         <v>187</v>
       </c>
-      <c r="O23" s="8">
-        <f>D42</f>
-        <v>8</v>
-      </c>
-      <c r="P23" s="8">
-        <f>E42</f>
-        <v>3</v>
-      </c>
-      <c r="Q23" s="8">
-        <f>F42</f>
-        <v>2</v>
-      </c>
-      <c r="R23" s="8">
-        <f>I42</f>
-        <v>3972</v>
-      </c>
-      <c r="S23" s="8">
-        <f>G42</f>
-        <v>0</v>
-      </c>
-      <c r="T23" s="8">
-        <f>L42</f>
-        <v>0</v>
-      </c>
-      <c r="U23" s="8">
-        <f>H42</f>
-        <v>3</v>
-      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A17)</f>
-        <v>ilevkivskyi/com2ann</v>
+        <f>CLEAN(RepositoriosPython!A36)</f>
+        <v>gvanrossum/pegen</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B17)</f>
-        <v>https://github.com/ilevkivskyi/com2ann</v>
+        <f>CLEAN(RepositoriosPython!B36)</f>
+        <v>https://github.com/gvanrossum/pegen</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C17)</f>
+        <f>CLEAN(RepositoriosPython!C36)</f>
         <v>Python</v>
       </c>
       <c r="D24" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D17))</f>
-        <v>50</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D36))</f>
+        <v>145</v>
       </c>
       <c r="E24" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E17))</f>
-        <v>6</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E36))</f>
+        <v>17</v>
       </c>
       <c r="F24" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F17))</f>
-        <v>1</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F36))</f>
+        <v>19</v>
       </c>
       <c r="G24" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G17))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G36))</f>
         <v>0</v>
       </c>
       <c r="H24" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H17,1,11)))</f>
-        <v>42622</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H36,1,11)))</f>
+        <v>43592</v>
       </c>
       <c r="I24" s="2">
-        <f>VALUE(CLEAN(M24))</f>
-        <v>1648</v>
+        <f t="shared" si="0"/>
+        <v>16377</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="0"/>
-        <v>1282</v>
+        <f t="shared" si="1"/>
+        <v>312</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24" t="s">
@@ -3705,832 +3667,146 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A19)</f>
-        <v>gvanrossum/pytype</v>
+        <f>CLEAN(RepositoriosPython!A40)</f>
+        <v>gvanrossum/guidos_time_machine</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B19)</f>
-        <v>https://github.com/gvanrossum/pytype</v>
+        <f>CLEAN(RepositoriosPython!B40)</f>
+        <v>https://github.com/gvanrossum/guidos_time_machine</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C19)</f>
+        <f>CLEAN(RepositoriosPython!C40)</f>
         <v>Python</v>
       </c>
       <c r="D25" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D19))</f>
-        <v>4</v>
+        <f>VALUE(CLEAN(RepositoriosPython!D40))</f>
+        <v>49</v>
       </c>
       <c r="E25" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E19))</f>
-        <v>1</v>
+        <f>VALUE(CLEAN(RepositoriosPython!E40))</f>
+        <v>10</v>
       </c>
       <c r="F25" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F19))</f>
-        <v>1</v>
+        <f>VALUE(CLEAN(RepositoriosPython!F40))</f>
+        <v>2</v>
       </c>
       <c r="G25" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G19))</f>
+        <f>VALUE(CLEAN(RepositoriosPython!G40))</f>
         <v>0</v>
       </c>
       <c r="H25" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H19,1,11)))</f>
-        <v>42776</v>
+        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H40,1,11)))</f>
+        <v>43895</v>
       </c>
       <c r="I25" s="2">
-        <f>VALUE(CLEAN(M25))</f>
-        <v>51569</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="0"/>
-        <v>1128</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A20)</f>
-        <v>gvanrossum/arq</v>
-      </c>
-      <c r="B26" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B20)</f>
-        <v>https://github.com/gvanrossum/arq</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C20)</f>
-        <v>Python</v>
-      </c>
-      <c r="D26" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D20))</f>
-        <v>3</v>
-      </c>
-      <c r="E26" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E20))</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F20))</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G20))</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H20,1,11)))</f>
-        <v>42783</v>
-      </c>
-      <c r="I26" s="2">
-        <f>VALUE(CLEAN(M26))</f>
-        <v>1645</v>
-      </c>
-      <c r="K26" s="9">
-        <f t="shared" si="0"/>
-        <v>1121</v>
-      </c>
-      <c r="L26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A21)</f>
-        <v>emilyemorehouse/cpython</v>
-      </c>
-      <c r="B27" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B21)</f>
-        <v>https://github.com/emilyemorehouse/cpython</v>
-      </c>
-      <c r="C27" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C21)</f>
-        <v>Python</v>
-      </c>
-      <c r="D27" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D21))</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E21))</f>
-        <v>2</v>
-      </c>
-      <c r="F27" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F21))</f>
-        <v>1</v>
-      </c>
-      <c r="G27" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G21))</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H21,1,11)))</f>
-        <v>42786</v>
-      </c>
-      <c r="I27" s="2">
-        <f>VALUE(CLEAN(M27))</f>
-        <v>740970</v>
-      </c>
-      <c r="K27" s="9">
-        <f t="shared" si="0"/>
-        <v>1118</v>
-      </c>
-      <c r="L27" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M27" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A22)</f>
-        <v>neogeny/TatSu</v>
-      </c>
-      <c r="B28" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B22)</f>
-        <v>https://github.com/neogeny/TatSu</v>
-      </c>
-      <c r="C28" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C22)</f>
-        <v>Python</v>
-      </c>
-      <c r="D28" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D22))</f>
-        <v>146</v>
-      </c>
-      <c r="E28" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E22))</f>
-        <v>13</v>
-      </c>
-      <c r="F28" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F22))</f>
-        <v>34</v>
-      </c>
-      <c r="G28" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G22))</f>
-        <v>13</v>
-      </c>
-      <c r="H28" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H22,1,11)))</f>
-        <v>42857</v>
-      </c>
-      <c r="I28" s="2">
-        <f>VALUE(CLEAN(M28))</f>
-        <v>11608</v>
-      </c>
-      <c r="K28" s="9">
-        <f t="shared" si="0"/>
-        <v>1047</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="1"/>
-        <v>1.2416427889207259E-2</v>
-      </c>
-      <c r="M28" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A24)</f>
-        <v>gvanrossum/mypy</v>
-      </c>
-      <c r="B29" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B24)</f>
-        <v>https://github.com/gvanrossum/mypy</v>
-      </c>
-      <c r="C29" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C24)</f>
-        <v>Python</v>
-      </c>
-      <c r="D29" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D24))</f>
-        <v>15</v>
-      </c>
-      <c r="E29" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E24))</f>
-        <v>4</v>
-      </c>
-      <c r="F29" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F24))</f>
-        <v>5</v>
-      </c>
-      <c r="G29" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G24))</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H24,1,11)))</f>
-        <v>42892</v>
-      </c>
-      <c r="I29" s="2">
-        <f>VALUE(CLEAN(M29))</f>
-        <v>94773</v>
-      </c>
-      <c r="K29" s="9">
-        <f t="shared" si="0"/>
-        <v>1012</v>
-      </c>
-      <c r="L29" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A25)</f>
-        <v>gvanrossum/mypy-dummy</v>
-      </c>
-      <c r="B30" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B25)</f>
-        <v>https://github.com/gvanrossum/mypy-dummy</v>
-      </c>
-      <c r="C30" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C25)</f>
-        <v>Python</v>
-      </c>
-      <c r="D30" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D25))</f>
-        <v>6</v>
-      </c>
-      <c r="E30" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E25))</f>
-        <v>2</v>
-      </c>
-      <c r="F30" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F25))</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G25))</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H25,1,11)))</f>
-        <v>42978</v>
-      </c>
-      <c r="I30" s="2">
-        <f>VALUE(CLEAN(M30))</f>
-        <v>35</v>
-      </c>
-      <c r="K30" s="9">
-        <f t="shared" si="0"/>
-        <v>926</v>
-      </c>
-      <c r="L30" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A26)</f>
-        <v>gvanrossum/pep550</v>
-      </c>
-      <c r="B31" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B26)</f>
-        <v>https://github.com/gvanrossum/pep550</v>
-      </c>
-      <c r="C31" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C26)</f>
-        <v>Python</v>
-      </c>
-      <c r="D31" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D26))</f>
-        <v>7</v>
-      </c>
-      <c r="E31" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E26))</f>
-        <v>3</v>
-      </c>
-      <c r="F31" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F26))</f>
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G26))</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H26,1,11)))</f>
-        <v>42983</v>
-      </c>
-      <c r="I31" s="2">
-        <f>VALUE(CLEAN(M31))</f>
-        <v>390</v>
-      </c>
-      <c r="K31" s="9">
-        <f t="shared" si="0"/>
-        <v>921</v>
-      </c>
-      <c r="L31" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M31" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A27)</f>
-        <v>gvanrossum/welcome-wagon-2018</v>
-      </c>
-      <c r="B32" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B27)</f>
-        <v>https://github.com/gvanrossum/welcome-wagon-2018</v>
-      </c>
-      <c r="C32" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C27)</f>
-        <v>Python</v>
-      </c>
-      <c r="D32" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D27))</f>
-        <v>2</v>
-      </c>
-      <c r="E32" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E27))</f>
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F27))</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G27))</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H27,1,11)))</f>
-        <v>43124</v>
-      </c>
-      <c r="I32" s="2">
-        <f>VALUE(CLEAN(M32))</f>
-        <v>291</v>
-      </c>
-      <c r="K32" s="9">
-        <f t="shared" si="0"/>
-        <v>780</v>
-      </c>
-      <c r="L32" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M32" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A28)</f>
-        <v>gvanrossum/cpython</v>
-      </c>
-      <c r="B33" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B28)</f>
-        <v>https://github.com/gvanrossum/cpython</v>
-      </c>
-      <c r="C33" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C28)</f>
-        <v>Python</v>
-      </c>
-      <c r="D33" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D28))</f>
-        <v>59</v>
-      </c>
-      <c r="E33" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E28))</f>
-        <v>6</v>
-      </c>
-      <c r="F33" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F28))</f>
-        <v>3</v>
-      </c>
-      <c r="G33" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G28))</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H28,1,11)))</f>
-        <v>43298</v>
-      </c>
-      <c r="I33" s="2">
-        <f>VALUE(CLEAN(M33))</f>
-        <v>755749</v>
-      </c>
-      <c r="K33" s="9">
-        <f t="shared" si="0"/>
-        <v>606</v>
-      </c>
-      <c r="L33" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M33" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A32)</f>
-        <v>gvanrossum/python-memcached</v>
-      </c>
-      <c r="B34" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B32)</f>
-        <v>https://github.com/gvanrossum/python-memcached</v>
-      </c>
-      <c r="C34" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C32)</f>
-        <v>Python</v>
-      </c>
-      <c r="D34" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D32))</f>
-        <v>5</v>
-      </c>
-      <c r="E34" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E32))</f>
-        <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F32))</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G32))</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H32,1,11)))</f>
-        <v>43458</v>
-      </c>
-      <c r="I34" s="2">
-        <f>VALUE(CLEAN(M34))</f>
-        <v>1893</v>
-      </c>
-      <c r="K34" s="9">
-        <f t="shared" si="0"/>
-        <v>446</v>
-      </c>
-      <c r="L34" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A33)</f>
-        <v>python/mypy_extensions</v>
-      </c>
-      <c r="B35" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B33)</f>
-        <v>https://github.com/python/mypy_extensions</v>
-      </c>
-      <c r="C35" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C33)</f>
-        <v>Python</v>
-      </c>
-      <c r="D35" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D33))</f>
-        <v>68</v>
-      </c>
-      <c r="E35" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E33))</f>
-        <v>13</v>
-      </c>
-      <c r="F35" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F33))</f>
-        <v>12</v>
-      </c>
-      <c r="G35" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G33))</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H33,1,11)))</f>
-        <v>43479</v>
-      </c>
-      <c r="I35" s="2">
-        <f>VALUE(CLEAN(M35))</f>
-        <v>355</v>
-      </c>
-      <c r="K35" s="9">
-        <f t="shared" si="0"/>
-        <v>425</v>
-      </c>
-      <c r="L35" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M35" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A34)</f>
-        <v>gvanrossum/stone</v>
-      </c>
-      <c r="B36" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B34)</f>
-        <v>https://github.com/gvanrossum/stone</v>
-      </c>
-      <c r="C36" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C34)</f>
-        <v>Python</v>
-      </c>
-      <c r="D36" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D34))</f>
-        <v>3</v>
-      </c>
-      <c r="E36" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E34))</f>
-        <v>1</v>
-      </c>
-      <c r="F36" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F34))</f>
-        <v>1</v>
-      </c>
-      <c r="G36" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G34))</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H34,1,11)))</f>
-        <v>43532</v>
-      </c>
-      <c r="I36" s="2">
-        <f>VALUE(CLEAN(M36))</f>
-        <v>29451</v>
-      </c>
-      <c r="K36" s="9">
-        <f t="shared" si="0"/>
-        <v>372</v>
-      </c>
-      <c r="L36" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A35)</f>
-        <v>neogeny/pygl</v>
-      </c>
-      <c r="B37" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B35)</f>
-        <v>https://github.com/neogeny/pygl</v>
-      </c>
-      <c r="C37" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C35)</f>
-        <v>Python</v>
-      </c>
-      <c r="D37" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D35))</f>
-        <v>3</v>
-      </c>
-      <c r="E37" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E35))</f>
-        <v>2</v>
-      </c>
-      <c r="F37" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F35))</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G35))</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H35,1,11)))</f>
-        <v>43582</v>
-      </c>
-      <c r="I37" s="2">
-        <f>VALUE(CLEAN(M37))</f>
-        <v>4561</v>
-      </c>
-      <c r="K37" s="9">
-        <f t="shared" si="0"/>
-        <v>322</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A36)</f>
-        <v>gvanrossum/pegen</v>
-      </c>
-      <c r="B38" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B36)</f>
-        <v>https://github.com/gvanrossum/pegen</v>
-      </c>
-      <c r="C38" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C36)</f>
-        <v>Python</v>
-      </c>
-      <c r="D38" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D36))</f>
-        <v>145</v>
-      </c>
-      <c r="E38" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E36))</f>
-        <v>17</v>
-      </c>
-      <c r="F38" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F36))</f>
-        <v>19</v>
-      </c>
-      <c r="G38" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G36))</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H36,1,11)))</f>
-        <v>43592</v>
-      </c>
-      <c r="I38" s="2">
-        <f>VALUE(CLEAN(M38))</f>
-        <v>16377</v>
-      </c>
-      <c r="K38" s="9">
-        <f t="shared" si="0"/>
-        <v>312</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!A40)</f>
-        <v>gvanrossum/guidos_time_machine</v>
-      </c>
-      <c r="B39" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!B40)</f>
-        <v>https://github.com/gvanrossum/guidos_time_machine</v>
-      </c>
-      <c r="C39" s="2" t="str">
-        <f>CLEAN(RepositoriosPython!C40)</f>
-        <v>Python</v>
-      </c>
-      <c r="D39" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!D40))</f>
-        <v>49</v>
-      </c>
-      <c r="E39" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!E40))</f>
-        <v>10</v>
-      </c>
-      <c r="F39" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!F40))</f>
-        <v>2</v>
-      </c>
-      <c r="G39" s="2">
-        <f>VALUE(CLEAN(RepositoriosPython!G40))</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="3">
-        <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H40,1,11)))</f>
-        <v>43895</v>
-      </c>
-      <c r="I39" s="2">
-        <f>VALUE(CLEAN(M39))</f>
-        <v>26</v>
-      </c>
-      <c r="K39" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="str">
         <f>CLEAN(RepositoriosPython!A30)</f>
         <v>mypyc/mypy_mypyc-wheels</v>
       </c>
-      <c r="B40" s="2" t="str">
+      <c r="B26" s="2" t="str">
         <f>CLEAN(RepositoriosPython!B30)</f>
         <v>https://github.com/mypyc/mypy_mypyc-wheels</v>
       </c>
-      <c r="C40" s="2" t="str">
+      <c r="C26" s="2" t="str">
         <f>CLEAN(RepositoriosPython!C30)</f>
         <v>Shell</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D26" s="4">
         <f>VALUE(CLEAN(RepositoriosPython!D30))</f>
         <v>4</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E26" s="4">
         <f>VALUE(CLEAN(RepositoriosPython!E30))</f>
         <v>2</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F26" s="4">
         <f>VALUE(CLEAN(RepositoriosPython!F30))</f>
         <v>0</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G26" s="4">
         <f>VALUE(CLEAN(RepositoriosPython!G30))</f>
         <v>1147</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H26" s="3">
         <f>DATEVALUE(CLEAN(MID(RepositoriosPython!H30,1,11)))</f>
         <v>43383</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C42" s="5" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="2">
-        <f>MEDIAN(D15:D39)</f>
-        <v>8</v>
-      </c>
-      <c r="E42" s="2">
-        <f t="shared" ref="E42:G42" si="2">MEDIAN(E15:E39)</f>
+      <c r="D28" s="2">
+        <f>MEDIAN(D15:D25)</f>
+        <v>49</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" ref="E28:G28" si="3">MEDIAN(E15:E25)</f>
+        <v>6</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F42" s="2">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G42" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H42" s="6">
-        <f>2020-YEAR(MEDIAN(H15:H39))</f>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="6">
+        <f>2020-YEAR(MEDIAN(H15:H25))</f>
         <v>3</v>
       </c>
-      <c r="I42" s="2">
-        <f>MEDIAN(I15:I39)</f>
-        <v>3972</v>
-      </c>
-      <c r="L42" s="2">
-        <f>MEDIAN(L15:L39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H43" s="9">
-        <f>_xlfn.DAYS("14/03/2020",MEDIAN(H15:H39))</f>
-        <v>1118</v>
+      <c r="I28" s="2">
+        <f>MEDIAN(I15:I25)</f>
+        <v>1648</v>
+      </c>
+      <c r="L28" s="2">
+        <f>MEDIAN(L15:L25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H29" s="9">
+        <f>_xlfn.DAYS("14/03/2020",MEDIAN(H15:H25))</f>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H40" xr:uid="{DFC49859-5E81-4363-B397-7F46F3A3FCE8}">
+  <autoFilter ref="A1:H26" xr:uid="{DFC49859-5E81-4363-B397-7F46F3A3FCE8}">
     <filterColumn colId="2">
       <filters>
         <filter val="Python"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H40">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H26">
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
   <mergeCells count="3">
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="O20:U20"/>
-    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="S17:T17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H42" formula="1"/>
+    <ignoredError sqref="H28" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>